<commit_message>
final version of initial report
</commit_message>
<xml_diff>
--- a/Project Management/v1/figs/Timetable.xlsx
+++ b/Project Management/v1/figs/Timetable.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villancikos/Downloads/v1/figs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Desktop\Group project\v1\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="645" yWindow="1185" windowWidth="28155" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$4:$X$16</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -83,8 +83,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,27 +100,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="6">
@@ -273,69 +278,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,6 +354,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -355,14 +365,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>11399</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>49502</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>153865</xdr:rowOff>
+      <xdr:rowOff>115765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>125699</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>191471</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:to>
@@ -371,7 +381,7 @@
         <xdr:cNvPr id="2" name="Grupo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92CBB0E0-5B76-4E7A-95FC-85CC80C571BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92CBB0E0-5B76-4E7A-95FC-85CC80C571BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -379,10 +389,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2766653" y="541323"/>
-          <a:ext cx="1491927" cy="2565665"/>
-          <a:chOff x="19821525" y="4154365"/>
-          <a:chExt cx="1485900" cy="2520462"/>
+          <a:off x="2249777" y="496765"/>
+          <a:ext cx="1913619" cy="2558562"/>
+          <a:chOff x="19526482" y="4116265"/>
+          <a:chExt cx="2195384" cy="2558562"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -390,7 +400,7 @@
           <xdr:cNvPr id="3" name="Grupo 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{148B7933-0899-4CA7-81CD-4ED1C33C2DCF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148B7933-0899-4CA7-81CD-4ED1C33C2DCF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -409,7 +419,7 @@
             <xdr:cNvPr id="5" name="Triángulo isósceles 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1B70D0E1-4478-4A43-AE4A-ECA9628B2E9C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B70D0E1-4478-4A43-AE4A-ECA9628B2E9C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -460,7 +470,7 @@
             <xdr:cNvPr id="6" name="Conector recto 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7D1D698-3FC5-4BB1-8954-03ED9AD99D5A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7D1D698-3FC5-4BB1-8954-03ED9AD99D5A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -504,7 +514,7 @@
           <xdr:cNvPr id="4" name="CuadroTexto 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2BC516DF-F137-4263-96E2-64B73E358C3A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BC516DF-F137-4263-96E2-64B73E358C3A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -512,8 +522,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="19821525" y="4154365"/>
-            <a:ext cx="1485900" cy="189035"/>
+            <a:off x="19526482" y="4116265"/>
+            <a:ext cx="2195384" cy="274760"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -542,26 +552,29 @@
           <a:lstStyle/>
           <a:p>
             <a:r>
-              <a:rPr lang="en-US" sz="900" b="1" i="1">
+              <a:rPr lang="en-US" sz="1000" b="0" i="1">
                 <a:solidFill>
                   <a:srgbClr val="C00000"/>
                 </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
               </a:rPr>
               <a:t>Current Situation</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="900" b="1" i="1" baseline="0">
+              <a:rPr lang="en-US" sz="1000" b="0" i="1" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="C00000"/>
                 </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="900" b="1" i="1">
+              <a:rPr lang="en-US" sz="1000" b="0" i="1">
                 <a:solidFill>
                   <a:srgbClr val="C00000"/>
                 </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
               </a:rPr>
               <a:t>(08/02/2017)</a:t>
             </a:r>
@@ -837,18 +850,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W17"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.42578125" customWidth="1"/>
+    <col min="18" max="19" width="5.7109375" customWidth="1"/>
+    <col min="20" max="21" width="5.85546875" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -871,7 +887,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -894,399 +910,510 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="28" t="str">
+      <c r="F5" s="16" t="str">
         <f>"26/01/2017"</f>
         <v>26/01/2017</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
+      <c r="K5" s="18"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
-      <c r="R5" s="14" t="str">
+      <c r="R5" s="19" t="str">
         <f>"07/03/2017"</f>
         <v>07/03/2017</v>
       </c>
-      <c r="S5" s="13"/>
-      <c r="T5" s="30" t="s">
+      <c r="S5" s="20"/>
+      <c r="T5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="30"/>
-      <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
+      <c r="U5" s="21"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="10"/>
-      <c r="W6" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="17" t="s">
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="9"/>
-      <c r="W7" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="17" t="s">
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="8"/>
-      <c r="W8" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="20" t="s">
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="17" t="s">
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="17" t="s">
+      <c r="H10" s="23"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="20" t="s">
+      <c r="J11" s="23"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="23" t="s">
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="1"/>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="25" t="s">
+      <c r="P13" s="30"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="R14" s="26"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="20" t="s">
+      <c r="R14" s="32"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="17" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="18"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="G15:R15"/>
     <mergeCell ref="S16:U16"/>
@@ -1296,10 +1423,15 @@
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D7:F7"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>